<commit_message>
amélioration lcp minifier css
</commit_message>
<xml_diff>
--- a/Audit-SEO.xlsx
+++ b/Audit-SEO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="97">
   <si>
     <t xml:space="preserve">Catégorie</t>
   </si>
@@ -113,7 +113,7 @@
 Et peuvent ralentir l’affichage</t>
   </si>
   <si>
-    <t xml:space="preserve">Désigner ces balises en « refer » 
+    <t xml:space="preserve">Désigner ces balises en « defer » 
 Pour qu’elles ne soient pas prioritaires</t>
   </si>
   <si>
@@ -368,14 +368,16 @@
 Déjà venus une première fois</t>
   </si>
   <si>
-    <t xml:space="preserve">Fichier lié aux html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un fichier bootstrap inexistant était lié à la page contact,
-Cela ne mettait pas le style voulu sur la page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toujours lier des fichiers existants</t>
+    <t xml:space="preserve">Sécurité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bootstrap et Jquery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bootstrap et Jquery ne sont pas à jour, créant des failles de sécurité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utiliser des logiciels sur leur dernière version</t>
   </si>
   <si>
     <t xml:space="preserve">La checklist donnée en relation avec la documentation MDN est aussi traitée</t>
@@ -452,7 +454,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,6 +483,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD4EA6B"/>
         <bgColor rgb="FFFFE994"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6D6D"/>
+        <bgColor rgb="FFFF6600"/>
       </patternFill>
     </fill>
   </fills>
@@ -525,7 +533,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -582,6 +590,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -594,7 +614,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -634,7 +654,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF6D6D"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -681,11 +701,11 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.37109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.4140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.74"/>
@@ -1029,7 +1049,9 @@
       <c r="D16" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="10"/>
+      <c r="E16" s="10" t="s">
+        <v>10</v>
+      </c>
       <c r="F16" s="4" t="s">
         <v>11</v>
       </c>
@@ -1223,54 +1245,52 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="68.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B27" s="11" t="s">
+      <c r="A27" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="B27" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="C27" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="12"/>
+      <c r="D27" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="16"/>
+      <c r="F27" s="15"/>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="16"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="19"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="18"/>
+      <c r="B29" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="21"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E30" s="18"/>
+      <c r="E30" s="21"/>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E31" s="18"/>
+      <c r="E31" s="21"/>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E32" s="18"/>
+      <c r="E32" s="21"/>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E33" s="18"/>
+      <c r="E33" s="21"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E34" s="18"/>
+      <c r="E34" s="21"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E35" s="18"/>
+      <c r="E35" s="21"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>